<commit_message>
Added a new testcase for test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestDataFile.xlsx
+++ b/src/test/resources/TestData/TestDataFile.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajasekhar/IdeaProjects/FrameWorkSkeleton/src/test/resources/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raj Projects\frameworkskeletonOnMac-master\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92750482-08CA-B046-A9DC-6123B03DE3A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E35FB-7D9D-4833-9940-3B216375512E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="18240" windowHeight="8800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CustomerInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>password</t>
   </si>
@@ -34,16 +35,87 @@
   </si>
   <si>
     <t>emailid</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>rajasekhar.rct@gmail.com</t>
+  </si>
+  <si>
+    <t>Welcome123</t>
+  </si>
+  <si>
+    <t>Maddigalla</t>
+  </si>
+  <si>
+    <t>Rajasekhar</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>ISSI</t>
+  </si>
+  <si>
+    <t>NewsLetter</t>
+  </si>
+  <si>
+    <t>Your Store Name</t>
+  </si>
+  <si>
+    <t>CustomerRole</t>
+  </si>
+  <si>
+    <t>Administrators</t>
+  </si>
+  <si>
+    <t>ManagerOfVendor</t>
+  </si>
+  <si>
+    <t>Vendor 2</t>
+  </si>
+  <si>
+    <t>07/29/1990</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +138,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,13 +494,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -425,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -440,23 +526,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2BD1DC2C-AE4D-4252-AFF6-8D2180521031}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E5EEB7-4692-4873-AE45-812456E305A3}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>